<commit_message>
dataset generation from hierarchy assemblies complete
</commit_message>
<xml_diff>
--- a/files/interesting_dengue_communities.xlsx
+++ b/files/interesting_dengue_communities.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idekeradmin/Dropbox/GitHub/agent_evaluation/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64E1D07B-839C-7E40-A004-F007842B0EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF1EA07-CE56-D740-852A-9D95990E9593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15880" yWindow="-25920" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{A80CA0BE-16C8-3241-85E2-3B10CFCF48C3}"/>
+    <workbookView xWindow="8580" yWindow="-27800" windowWidth="29200" windowHeight="18880" activeTab="1" xr2:uid="{A80CA0BE-16C8-3241-85E2-3B10CFCF48C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Top 20 communities" sheetId="1" r:id="rId1"/>
     <sheet name="Top 10 communities" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Top 10 communities'!$A$1:$A$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Top 10 communities'!$A$1:$A$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Top 20 communities'!$A$1:$A$18</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Community</t>
   </si>
@@ -101,6 +101,21 @@
   </si>
   <si>
     <t>Epidermal growth factor signalling in viral infection and tissue repair</t>
+  </si>
+  <si>
+    <t>Endothelial Barrier Function and Viral Entry Modulation</t>
+  </si>
+  <si>
+    <t>Transcriptional regulation and chromatin remodelling</t>
+  </si>
+  <si>
+    <t>Chromatin remodelling and transcriptional regulation</t>
+  </si>
+  <si>
+    <t>RNA metabolism and modification in viral infection</t>
+  </si>
+  <si>
+    <t>RNA metabolism and viral defense mechanism</t>
   </si>
 </sst>
 </file>
@@ -633,10 +648,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E787B99D-1B79-2F42-86C9-95510D44E692}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -651,58 +666,68 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A10" xr:uid="{64FF2794-78BF-5047-9F29-A6D5617BC0C9}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A12">
-      <sortCondition ref="A1:A12"/>
+  <autoFilter ref="A1:A12" xr:uid="{64FF2794-78BF-5047-9F29-A6D5617BC0C9}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A14">
+      <sortCondition ref="A1:A14"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>